<commit_message>
fix the tag for an indicator
20120905_extreme_poverty_percent_people_below_125_a_day
</commit_message>
<xml_diff>
--- a/etl/source/graph_settings.xlsx
+++ b/etl/source/graph_settings.xlsx
@@ -8360,9 +8360,6 @@
     <t>co2_intensity_of_economic_output_kg_co2_per_2011_ppp_of_gdp</t>
   </si>
   <si>
-    <t>20120905_extreme_poverty_percent_people_below_190_a_day</t>
-  </si>
-  <si>
     <t>Extreme poverty (% people below $1.90 a day) version 20120905</t>
   </si>
   <si>
@@ -8382,6 +8379,9 @@
   </si>
   <si>
     <t>Extreme poverty (% people below $1.90 a day)</t>
+  </si>
+  <si>
+    <t>20120905_extreme_poverty_percent_people_below_125_a_day</t>
   </si>
 </sst>
 </file>
@@ -8538,8 +8538,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
@@ -8673,8 +8674,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9291,10 +9293,10 @@
   <dimension ref="A1:L562"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G436" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomRight" activeCell="G526" sqref="G526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -10371,7 +10373,7 @@
     </row>
     <row r="35" spans="1:10" ht="38.25" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>237</v>
@@ -10389,7 +10391,7 @@
         <v>63</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>76</v>
@@ -11009,7 +11011,7 @@
     </row>
     <row r="55" spans="1:10" ht="25.5" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>332</v>
@@ -11027,7 +11029,7 @@
         <v>63</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>65</v>
@@ -11105,7 +11107,7 @@
     </row>
     <row r="58" spans="1:10" ht="25.5" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>347</v>
@@ -11123,7 +11125,7 @@
         <v>63</v>
       </c>
       <c r="G58" s="44" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="H58" s="11" t="s">
         <v>65</v>
@@ -25833,7 +25835,7 @@
     </row>
     <row r="526" spans="1:10" ht="38.25" customHeight="1">
       <c r="A526" s="8" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="B526" s="8" t="s">
         <v>2679</v>
@@ -25851,7 +25853,7 @@
         <v>63</v>
       </c>
       <c r="G526" s="44" t="s">
-        <v>2778</v>
+        <v>2785</v>
       </c>
       <c r="H526" s="11" t="s">
         <v>65</v>

</xml_diff>